<commit_message>
add vis results of toy data
</commit_message>
<xml_diff>
--- a/etc/toy_comb.xlsx
+++ b/etc/toy_comb.xlsx
@@ -822,7 +822,7 @@
         <v>-1.032814264297485</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.544162218325261</v>
+        <v>-1.025716894330972</v>
       </c>
       <c r="F4" t="n">
         <v>-1.538369297981262</v>
@@ -989,7 +989,7 @@
         <v>-1.158902525901794</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.5445167255194869</v>
+        <v>-1.089044612668089</v>
       </c>
       <c r="F5" t="n">
         <v>-1.538369297981262</v>
@@ -1156,7 +1156,7 @@
         <v>-1.151021957397461</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.5520408160718281</v>
+        <v>-1.161882250675194</v>
       </c>
       <c r="F6" t="n">
         <v>-1.538369297981262</v>
@@ -1323,7 +1323,7 @@
         <v>-1.135260939598083</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.5787087157052093</v>
+        <v>-1.17578158242377</v>
       </c>
       <c r="F7" t="n">
         <v>-1.538369297981262</v>
@@ -1490,7 +1490,7 @@
         <v>-1.139201164245605</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.6560893347534312</v>
+        <v>-1.210568185744106</v>
       </c>
       <c r="F8" t="n">
         <v>-1.538369297981262</v>
@@ -1657,7 +1657,7 @@
         <v>-0.8515626192092896</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.7218074399509758</v>
+        <v>-1.245516927606187</v>
       </c>
       <c r="F9" t="n">
         <v>-1.538369297981262</v>
@@ -1824,7 +1824,7 @@
         <v>-0.9067261815071106</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.7118755605092449</v>
+        <v>-1.291294673448375</v>
       </c>
       <c r="F10" t="n">
         <v>-1.538369297981262</v>
@@ -1991,7 +1991,7 @@
         <v>-0.8515626192092896</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.6997271567743862</v>
+        <v>-1.357943287741367</v>
       </c>
       <c r="F11" t="n">
         <v>-1.538369297981262</v>
@@ -2158,7 +2158,7 @@
         <v>-0.8594431281089783</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.7078487520371496</v>
+        <v>-1.410895716629916</v>
       </c>
       <c r="F12" t="n">
         <v>-1.538369297981262</v>
@@ -2325,7 +2325,7 @@
         <v>-0.7648770809173584</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.7583885026444857</v>
+        <v>-1.392359138468838</v>
       </c>
       <c r="F13" t="n">
         <v>-1.538369297981262</v>
@@ -2492,7 +2492,7 @@
         <v>-0.8791444301605225</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.7635540136703016</v>
+        <v>-1.422690822374978</v>
       </c>
       <c r="F14" t="n">
         <v>-1.538369297981262</v>
@@ -2659,7 +2659,7 @@
         <v>-1.115559697151184</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.7914464167977825</v>
+        <v>-1.429443019908541</v>
       </c>
       <c r="F15" t="n">
         <v>-1.538369297981262</v>
@@ -2826,7 +2826,7 @@
         <v>-1.024933815002441</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.8335556992718115</v>
+        <v>-1.424391699840141</v>
       </c>
       <c r="F16" t="n">
         <v>-1.538369297981262</v>
@@ -2993,7 +2993,7 @@
         <v>-1.020993590354919</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.8230504466341402</v>
+        <v>-1.423054635185899</v>
       </c>
       <c r="F17" t="n">
         <v>-1.553598284721375</v>
@@ -3160,7 +3160,7 @@
         <v>-1.024933815002441</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.8174202330887095</v>
+        <v>-1.397630849188016</v>
       </c>
       <c r="F18" t="n">
         <v>-1.593574523925781</v>
@@ -3327,7 +3327,7 @@
         <v>-0.9224872589111328</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.8256825692322295</v>
+        <v>-1.432065416297089</v>
       </c>
       <c r="F19" t="n">
         <v>-1.578345537185669</v>
@@ -3494,7 +3494,7 @@
         <v>-1.005232572555542</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.7865341026646541</v>
+        <v>-1.459020160250758</v>
       </c>
       <c r="F20" t="n">
         <v>-1.608803510665894</v>
@@ -3661,7 +3661,7 @@
         <v>-1.013113021850586</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.7610714118286083</v>
+        <v>-1.400988862462462</v>
       </c>
       <c r="F21" t="n">
         <v>-1.604044437408447</v>
@@ -3828,7 +3828,7 @@
         <v>-0.8870249390602112</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.7540010883819119</v>
+        <v>-1.400117499235842</v>
       </c>
       <c r="F22" t="n">
         <v>-1.614514350891113</v>
@@ -3995,7 +3995,7 @@
         <v>-0.8870249390602112</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.6902950993548272</v>
+        <v>-1.385556469793876</v>
       </c>
       <c r="F23" t="n">
         <v>-1.622128844261169</v>
@@ -4162,7 +4162,7 @@
         <v>-1.028874158859253</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.6545728346766932</v>
+        <v>-1.363868704889879</v>
       </c>
       <c r="F24" t="n">
         <v>-1.61641800403595</v>
@@ -4329,7 +4329,7 @@
         <v>-1.46624231338501</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.6511361705402325</v>
+        <v>-1.377523356750879</v>
       </c>
       <c r="F25" t="n">
         <v>-1.486971378326416</v>
@@ -4496,7 +4496,7 @@
         <v>-1.840566396713257</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.6998309906329946</v>
+        <v>-1.400907477746955</v>
       </c>
       <c r="F26" t="n">
         <v>-1.445091605186462</v>
@@ -4663,7 +4663,7 @@
         <v>-1.812984585762024</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.7553759538180976</v>
+        <v>-1.413350086176889</v>
       </c>
       <c r="F27" t="n">
         <v>-1.492682337760925</v>
@@ -4830,7 +4830,7 @@
         <v>-1.675075650215149</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.8421321131223322</v>
+        <v>-1.469552751423354</v>
       </c>
       <c r="F28" t="n">
         <v>-1.547887444496155</v>
@@ -4997,7 +4997,7 @@
         <v>-1.552927851676941</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.881241043962478</v>
+        <v>-1.539186418285493</v>
       </c>
       <c r="F29" t="n">
         <v>-1.505055904388428</v>
@@ -5164,7 +5164,7 @@
         <v>-1.044635057449341</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.9301631419138546</v>
+        <v>-1.598537851866019</v>
       </c>
       <c r="F30" t="n">
         <v>-1.511718511581421</v>
@@ -5331,7 +5331,7 @@
         <v>-0.9185469150543213</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.9572840200412964</v>
+        <v>-1.620577232388432</v>
       </c>
       <c r="F31" t="n">
         <v>-1.510766744613647</v>
@@ -5498,7 +5498,7 @@
         <v>-0.6781914830207825</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.8905149058982129</v>
+        <v>-1.624475076579431</v>
       </c>
       <c r="F32" t="n">
         <v>-1.500296831130981</v>
@@ -5665,7 +5665,7 @@
         <v>-0.6860719919204712</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.8446234422655592</v>
+        <v>-1.570375270409734</v>
       </c>
       <c r="F33" t="n">
         <v>-1.558357357978821</v>
@@ -5832,7 +5832,7 @@
         <v>-1.363795638084412</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.7671466126040445</v>
+        <v>-1.562883670654668</v>
       </c>
       <c r="F34" t="n">
         <v>-1.528851270675659</v>
@@ -5999,7 +5999,7 @@
         <v>-0.7333550453186035</v>
       </c>
       <c r="E35" t="n">
-        <v>-0.7869298805317951</v>
+        <v>-1.601642983692412</v>
       </c>
       <c r="F35" t="n">
         <v>-1.506959557533264</v>
@@ -6166,7 +6166,7 @@
         <v>-0.5875656604766846</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.7825700151005687</v>
+        <v>-1.530524098346381</v>
       </c>
       <c r="F36" t="n">
         <v>-1.51742947101593</v>
@@ -6333,7 +6333,7 @@
         <v>-0.6900122165679932</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.7404594708480047</v>
+        <v>-1.487778196027346</v>
       </c>
       <c r="F37" t="n">
         <v>-1.488875031471252</v>
@@ -6500,7 +6500,7 @@
         <v>-0.3275088369846344</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.7696246404985485</v>
+        <v>-1.435799755019596</v>
       </c>
       <c r="F38" t="n">
         <v>-1.46793520450592</v>
@@ -6667,7 +6667,7 @@
         <v>-0.4260152280330658</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.7046014072550426</v>
+        <v>-1.335343362104785</v>
       </c>
       <c r="F39" t="n">
         <v>-1.475549697875977</v>
@@ -6834,7 +6834,7 @@
         <v>-0.3866126537322998</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.643277393231486</v>
+        <v>-1.215414887393415</v>
       </c>
       <c r="F40" t="n">
         <v>-1.527899384498596</v>
@@ -7001,7 +7001,7 @@
         <v>-0.2999270856380463</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.5782918556217128</v>
+        <v>-1.099072176982056</v>
       </c>
       <c r="F41" t="n">
         <v>-1.560261011123657</v>
@@ -7168,7 +7168,7 @@
         <v>-0.1935402154922485</v>
       </c>
       <c r="E42" t="n">
-        <v>-0.4316692467982546</v>
+        <v>-1.111698163892407</v>
       </c>
       <c r="F42" t="n">
         <v>-1.537417531013489</v>
@@ -7335,7 +7335,7 @@
         <v>-0.3196283578872681</v>
       </c>
       <c r="E43" t="n">
-        <v>-0.2566566209375798</v>
+        <v>-1.004484841774528</v>
       </c>
       <c r="F43" t="n">
         <v>-1.531706690788269</v>
@@ -7502,7 +7502,7 @@
         <v>-0.3905529379844666</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.179184220644464</v>
+        <v>-0.895533104280069</v>
       </c>
       <c r="F44" t="n">
         <v>-1.575490117073059</v>
@@ -7669,7 +7669,7 @@
         <v>-0.1659584492444992</v>
       </c>
       <c r="E45" t="n">
-        <v>-0.1007244523606677</v>
+        <v>-0.8877425681604231</v>
       </c>
       <c r="F45" t="n">
         <v>-1.655442357063293</v>
@@ -7836,7 +7836,7 @@
         <v>-0.1501974314451218</v>
       </c>
       <c r="E46" t="n">
-        <v>0.03136754114092836</v>
+        <v>-0.7140586476711956</v>
       </c>
       <c r="F46" t="n">
         <v>-1.66020143032074</v>
@@ -8003,7 +8003,7 @@
         <v>-0.08321312069892883</v>
       </c>
       <c r="E47" t="n">
-        <v>0.1173662127313255</v>
+        <v>-0.5141642748416255</v>
       </c>
       <c r="F47" t="n">
         <v>-1.606899976730347</v>
@@ -8170,7 +8170,7 @@
         <v>0.2792902290821075</v>
       </c>
       <c r="E48" t="n">
-        <v>0.2150585746170353</v>
+        <v>-0.3767736263917195</v>
       </c>
       <c r="F48" t="n">
         <v>-1.532658457756042</v>
@@ -8337,7 +8337,7 @@
         <v>0.7245388627052307</v>
       </c>
       <c r="E49" t="n">
-        <v>0.4077067899036481</v>
+        <v>-0.1546102687769471</v>
       </c>
       <c r="F49" t="n">
         <v>-1.526947617530823</v>
@@ -8504,7 +8504,7 @@
         <v>1.063400745391846</v>
       </c>
       <c r="E50" t="n">
-        <v>0.5166832372277502</v>
+        <v>-0.00735507517108883</v>
       </c>
       <c r="F50" t="n">
         <v>-1.506007671356201</v>
@@ -8671,7 +8671,7 @@
         <v>1.477127313613892</v>
       </c>
       <c r="E51" t="n">
-        <v>0.6909376393371088</v>
+        <v>0.0009356772765212185</v>
       </c>
       <c r="F51" t="n">
         <v>-1.546935677528381</v>
@@ -8838,7 +8838,7 @@
         <v>1.173727869987488</v>
       </c>
       <c r="E52" t="n">
-        <v>0.8741591334758836</v>
+        <v>0.1083437864557396</v>
       </c>
       <c r="F52" t="n">
         <v>-1.56977915763855</v>
@@ -9005,7 +9005,7 @@
         <v>0.6260325312614441</v>
       </c>
       <c r="E53" t="n">
-        <v>0.8867063643760096</v>
+        <v>0.28670572457638</v>
       </c>
       <c r="F53" t="n">
         <v>-1.511718511581421</v>
@@ -9172,7 +9172,7 @@
         <v>0.9924761652946472</v>
       </c>
       <c r="E54" t="n">
-        <v>0.9269963199249036</v>
+        <v>0.3582601863875089</v>
       </c>
       <c r="F54" t="n">
         <v>-1.511718511581421</v>
@@ -9339,7 +9339,7 @@
         <v>0.8742685317993164</v>
       </c>
       <c r="E55" t="n">
-        <v>0.9412188772748591</v>
+        <v>0.5068224905509293</v>
       </c>
       <c r="F55" t="n">
         <v>-1.508863091468811</v>
@@ -9506,7 +9506,7 @@
         <v>0.8388062119483948</v>
       </c>
       <c r="E56" t="n">
-        <v>1.032184908086974</v>
+        <v>0.7038495768079518</v>
       </c>
       <c r="F56" t="n">
         <v>-1.497441411018372</v>
@@ -9673,7 +9673,7 @@
         <v>0.4802431762218475</v>
       </c>
       <c r="E57" t="n">
-        <v>1.05281519743044</v>
+        <v>0.7790914812393701</v>
       </c>
       <c r="F57" t="n">
         <v>-1.314693212509155</v>
@@ -9840,7 +9840,7 @@
         <v>0.7087778449058533</v>
       </c>
       <c r="E58" t="n">
-        <v>0.9676525066935777</v>
+        <v>0.9529771811459843</v>
       </c>
       <c r="F58" t="n">
         <v>-1.15574038028717</v>
@@ -10007,7 +10007,7 @@
         <v>0.720598578453064</v>
       </c>
       <c r="E59" t="n">
-        <v>0.9188675220096697</v>
+        <v>0.8653764714089981</v>
       </c>
       <c r="F59" t="n">
         <v>-1.112908840179443</v>
@@ -10174,7 +10174,7 @@
         <v>0.7875829339027405</v>
       </c>
       <c r="E60" t="n">
-        <v>0.8382670018624768</v>
+        <v>0.8812407603552891</v>
       </c>
       <c r="F60" t="n">
         <v>-1.0243901014328</v>
@@ -10341,7 +10341,7 @@
         <v>0.9845956563949585</v>
       </c>
       <c r="E61" t="n">
-        <v>0.833274669940588</v>
+        <v>0.7152044795666204</v>
       </c>
       <c r="F61" t="n">
         <v>-1.066269874572754</v>
@@ -10508,7 +10508,7 @@
         <v>0.7442401051521301</v>
       </c>
       <c r="E62" t="n">
-        <v>0.6887640680882762</v>
+        <v>0.7708473357363961</v>
       </c>
       <c r="F62" t="n">
         <v>-1.059607267379761</v>
@@ -10675,7 +10675,7 @@
         <v>0.2280669361352921</v>
       </c>
       <c r="E63" t="n">
-        <v>0.5640872578792201</v>
+        <v>0.8040027748556264</v>
       </c>
       <c r="F63" t="n">
         <v>-1.070077180862427</v>
@@ -10842,7 +10842,7 @@
         <v>0.1216800808906555</v>
       </c>
       <c r="E64" t="n">
-        <v>0.3513542358820475</v>
+        <v>0.7791260750008709</v>
       </c>
       <c r="F64" t="n">
         <v>-1.11195695400238</v>
@@ -11009,7 +11009,7 @@
         <v>0.1768436282873154</v>
       </c>
       <c r="E65" t="n">
-        <v>0.1168169973369194</v>
+        <v>0.7484692728255495</v>
       </c>
       <c r="F65" t="n">
         <v>-1.051992654800415</v>
@@ -11176,7 +11176,7 @@
         <v>0.5157054662704468</v>
       </c>
       <c r="E66" t="n">
-        <v>-0.04641628843861727</v>
+        <v>0.6480528888051188</v>
       </c>
       <c r="F66" t="n">
         <v>-0.9682331681251526</v>
@@ -11343,7 +11343,7 @@
         <v>0.4369003772735596</v>
       </c>
       <c r="E67" t="n">
-        <v>-0.01847684463012882</v>
+        <v>0.3490039893512638</v>
       </c>
       <c r="F67" t="n">
         <v>-1.032956480979919</v>
@@ -11510,7 +11510,7 @@
         <v>0.4408406615257263</v>
       </c>
       <c r="E68" t="n">
-        <v>0.006903416580061023</v>
+        <v>0.2762556484625616</v>
       </c>
       <c r="F68" t="n">
         <v>-0.9568114280700684</v>
@@ -11677,7 +11677,7 @@
         <v>0.4763029217720032</v>
       </c>
       <c r="E69" t="n">
-        <v>-0.1283869226372</v>
+        <v>0.06765258533271959</v>
       </c>
       <c r="F69" t="n">
         <v>-0.9520523548126221</v>
@@ -11844,7 +11844,7 @@
         <v>-0.4732982814311981</v>
       </c>
       <c r="E70" t="n">
-        <v>-0.2138668718144532</v>
+        <v>-0.06168660171132616</v>
       </c>
       <c r="F70" t="n">
         <v>-0.8701964020729065</v>
@@ -12011,7 +12011,7 @@
         <v>-0.08321312069892883</v>
       </c>
       <c r="E71" t="n">
-        <v>-0.1319925862361906</v>
+        <v>-0.1793159187790533</v>
       </c>
       <c r="F71" t="n">
         <v>-0.8958953619003296</v>
@@ -12178,7 +12178,7 @@
         <v>-0.04381058365106583</v>
       </c>
       <c r="E72" t="n">
-        <v>-0.121758405687119</v>
+        <v>-0.3487493936943852</v>
       </c>
       <c r="F72" t="n">
         <v>-0.9006544351577759</v>
@@ -12345,7 +12345,7 @@
         <v>0.2477681934833527</v>
       </c>
       <c r="E73" t="n">
-        <v>-0.1489819610428453</v>
+        <v>-0.2642099952667538</v>
       </c>
       <c r="F73" t="n">
         <v>-0.8939917087554932</v>
@@ -12512,7 +12512,7 @@
         <v>0.2320071756839752</v>
       </c>
       <c r="E74" t="n">
-        <v>-0.1495880221889579</v>
+        <v>-0.2898683406368812</v>
       </c>
       <c r="F74" t="n">
         <v>-0.8045212626457214</v>
@@ -12679,7 +12679,7 @@
         <v>0.2123059183359146</v>
       </c>
       <c r="E75" t="n">
-        <v>-0.2599098540195168</v>
+        <v>-0.1654305717425732</v>
       </c>
       <c r="F75" t="n">
         <v>-0.7426534295082092</v>
@@ -12846,7 +12846,7 @@
         <v>0.4920639395713806</v>
       </c>
       <c r="E76" t="n">
-        <v>-0.3163090412728062</v>
+        <v>-0.1134528667723021</v>
       </c>
       <c r="F76" t="n">
         <v>-0.5913150906562805</v>
@@ -13013,7 +13013,7 @@
         <v>0.2674694657325745</v>
       </c>
       <c r="E77" t="n">
-        <v>-0.2387378410916956</v>
+        <v>-0.0447960925102982</v>
       </c>
       <c r="F77" t="n">
         <v>-0.4580612480640411</v>
@@ -13180,7 +13180,7 @@
         <v>0.05863601341843605</v>
       </c>
       <c r="E78" t="n">
-        <v>0.08147280619585741</v>
+        <v>0.06192972306965218</v>
       </c>
       <c r="F78" t="n">
         <v>-0.4685311913490295</v>
@@ -13347,7 +13347,7 @@
         <v>0.3147525191307068</v>
       </c>
       <c r="E79" t="n">
-        <v>0.1689567357007252</v>
+        <v>0.1389058435209626</v>
       </c>
       <c r="F79" t="n">
         <v>-0.3762052953243256</v>
@@ -13514,7 +13514,7 @@
         <v>0.8821490406990051</v>
       </c>
       <c r="E80" t="n">
-        <v>0.4483430510862905</v>
+        <v>0.3903973965160571</v>
       </c>
       <c r="F80" t="n">
         <v>-0.3314700722694397</v>
@@ -13681,7 +13681,7 @@
         <v>1.083101987838745</v>
       </c>
       <c r="E81" t="n">
-        <v>0.6267012301583789</v>
+        <v>0.6061088993191731</v>
       </c>
       <c r="F81" t="n">
         <v>-0.3619281053543091</v>
@@ -13848,7 +13848,7 @@
         <v>0.7521206736564636</v>
       </c>
       <c r="E82" t="n">
-        <v>0.8889774605907756</v>
+        <v>0.7184498791068192</v>
       </c>
       <c r="F82" t="n">
         <v>-0.1249265819787979</v>
@@ -14015,7 +14015,7 @@
         <v>0.7481803894042969</v>
       </c>
       <c r="E83" t="n">
-        <v>0.9376106112576401</v>
+        <v>0.9031762544449888</v>
       </c>
       <c r="F83" t="n">
         <v>-0.06972140073776245</v>
@@ -14182,7 +14182,7 @@
         <v>0.6299727559089661</v>
       </c>
       <c r="E84" t="n">
-        <v>0.8268446991003977</v>
+        <v>0.9783496548167785</v>
       </c>
       <c r="F84" t="n">
         <v>-0.03735975921154022</v>
@@ -14349,7 +14349,7 @@
         <v>0.3265732824802399</v>
       </c>
       <c r="E85" t="n">
-        <v>0.8942111602315865</v>
+        <v>0.8638495616593465</v>
       </c>
       <c r="F85" t="n">
         <v>0.2729313671588898</v>
@@ -14516,7 +14516,7 @@
         <v>0.7481803894042969</v>
       </c>
       <c r="E86" t="n">
-        <v>0.9350347955266746</v>
+        <v>0.9978462361465589</v>
       </c>
       <c r="F86" t="n">
         <v>0.1901236027479172</v>
@@ -14683,7 +14683,7 @@
         <v>0.8427464962005615</v>
       </c>
       <c r="E87" t="n">
-        <v>0.9364918342899513</v>
+        <v>1.00989380274683</v>
       </c>
       <c r="F87" t="n">
         <v>0.3176665902137756</v>
@@ -14850,7 +14850,7 @@
         <v>0.7560608983039856</v>
       </c>
       <c r="E88" t="n">
-        <v>0.9056677413105327</v>
+        <v>1.093832463156543</v>
       </c>
       <c r="F88" t="n">
         <v>0.2948230803012848</v>
@@ -15017,7 +15017,7 @@
         <v>0.6654350757598877</v>
       </c>
       <c r="E89" t="n">
-        <v>0.8421429752255356</v>
+        <v>1.023313132911055</v>
       </c>
       <c r="F89" t="n">
         <v>0.1958345025777817</v>
@@ -15184,7 +15184,7 @@
         <v>0.8782087564468384</v>
       </c>
       <c r="E90" t="n">
-        <v>0.769931599964629</v>
+        <v>1.063413926827912</v>
       </c>
       <c r="F90" t="n">
         <v>0.2795940339565277</v>
@@ -15351,7 +15351,7 @@
         <v>0.9530735611915588</v>
       </c>
       <c r="E91" t="n">
-        <v>0.7667314141552672</v>
+        <v>1.028225657340606</v>
       </c>
       <c r="F91" t="n">
         <v>0.1615692228078842</v>
@@ -15518,7 +15518,7 @@
         <v>0.9491333365440369</v>
       </c>
       <c r="E92" t="n">
-        <v>0.8143949931662051</v>
+        <v>0.8520938864935026</v>
       </c>
       <c r="F92" t="n">
         <v>-0.09637217968702316</v>
@@ -15685,7 +15685,7 @@
         <v>0.976715087890625</v>
       </c>
       <c r="E93" t="n">
-        <v>0.8810569612820259</v>
+        <v>1.020231238839348</v>
       </c>
       <c r="F93" t="n">
         <v>-0.04973332583904266</v>
@@ -15852,7 +15852,7 @@
         <v>1.090982556343079</v>
       </c>
       <c r="E94" t="n">
-        <v>0.8160990250777056</v>
+        <v>1.159805289895838</v>
       </c>
       <c r="F94" t="n">
         <v>-0.03260068595409393</v>
@@ -16019,7 +16019,7 @@
         <v>1.232831597328186</v>
       </c>
       <c r="E95" t="n">
-        <v>0.8179003190846114</v>
+        <v>1.288337622140865</v>
       </c>
       <c r="F95" t="n">
         <v>0.05782155692577362</v>
@@ -16186,7 +16186,7 @@
         <v>1.260413408279419</v>
       </c>
       <c r="E96" t="n">
-        <v>0.836112777884514</v>
+        <v>1.308625864353139</v>
       </c>
       <c r="F96" t="n">
         <v>0.0178454052656889</v>
@@ -16353,7 +16353,7 @@
         <v>1.201309561729431</v>
       </c>
       <c r="E97" t="n">
-        <v>0.8267396034632544</v>
+        <v>1.229542948338902</v>
       </c>
       <c r="F97" t="n">
         <v>0.02070085518062115</v>
@@ -16520,7 +16520,7 @@
         <v>1.248592615127563</v>
       </c>
       <c r="E98" t="n">
-        <v>0.8081046065764479</v>
+        <v>1.244841592482779</v>
       </c>
       <c r="F98" t="n">
         <v>-0.05258877575397491</v>
@@ -16687,7 +16687,7 @@
         <v>1.134325385093689</v>
       </c>
       <c r="E99" t="n">
-        <v>0.7784290475085017</v>
+        <v>1.243808721603681</v>
       </c>
       <c r="F99" t="n">
         <v>-0.1972643882036209</v>
@@ -16854,7 +16854,7 @@
         <v>0.7757622003555298</v>
       </c>
       <c r="E100" t="n">
-        <v>0.9132587061252282</v>
+        <v>1.302638199463567</v>
       </c>
       <c r="F100" t="n">
         <v>-0.1363483369350433</v>
@@ -17021,7 +17021,7 @@
         <v>0.8782087564468384</v>
       </c>
       <c r="E101" t="n">
-        <v>1.031194306788797</v>
+        <v>1.472254461400629</v>
       </c>
       <c r="F101" t="n">
         <v>-0.1449146568775177</v>
@@ -17188,7 +17188,7 @@
         <v>1.228891372680664</v>
       </c>
       <c r="E102" t="n">
-        <v>1.073360316722795</v>
+        <v>1.569432122792275</v>
       </c>
       <c r="F102" t="n">
         <v>-0.09351674467325211</v>
@@ -17355,7 +17355,7 @@
         <v>1.323457360267639</v>
       </c>
       <c r="E103" t="n">
-        <v>1.1662686452931</v>
+        <v>1.595719806493781</v>
       </c>
       <c r="F103" t="n">
         <v>0.1092194765806198</v>
@@ -17522,7 +17522,7 @@
         <v>0.9215515851974487</v>
       </c>
       <c r="E104" t="n">
-        <v>1.205957468518284</v>
+        <v>1.474703468388828</v>
       </c>
       <c r="F104" t="n">
         <v>0.04544800519943237</v>
@@ -17689,7 +17689,7 @@
         <v>0.917611300945282</v>
       </c>
       <c r="E105" t="n">
-        <v>1.091828338250138</v>
+        <v>1.578054486411112</v>
       </c>
       <c r="F105" t="n">
         <v>0.0007127657299861312</v>
@@ -17856,7 +17856,7 @@
         <v>1.035818934440613</v>
       </c>
       <c r="E106" t="n">
-        <v>1.009874560624171</v>
+        <v>1.576201669780694</v>
       </c>
       <c r="F106" t="n">
         <v>0.02926717512309551</v>
@@ -18023,7 +18023,7 @@
         <v>0.9688346385955811</v>
       </c>
       <c r="E107" t="n">
-        <v>1.015747929408115</v>
+        <v>1.561606467170072</v>
       </c>
       <c r="F107" t="n">
         <v>0.09589411318302155</v>
@@ -18190,7 +18190,7 @@
         <v>1.090982556343079</v>
       </c>
       <c r="E108" t="n">
-        <v>1.047799838050288</v>
+        <v>1.528300560960545</v>
       </c>
       <c r="F108" t="n">
         <v>0.3100520968437195</v>
@@ -18357,7 +18357,7 @@
         <v>0.858507513999939</v>
       </c>
       <c r="E109" t="n">
-        <v>0.9594003699265489</v>
+        <v>1.575446179882871</v>
       </c>
       <c r="F109" t="n">
         <v>0.2786422371864319</v>
@@ -18524,7 +18524,7 @@
         <v>0.8900295495986938</v>
       </c>
       <c r="E110" t="n">
-        <v>0.9255281354512345</v>
+        <v>1.488110075619492</v>
       </c>
       <c r="F110" t="n">
         <v>0.2805458605289459</v>
@@ -18691,7 +18691,7 @@
         <v>1.016117691993713</v>
       </c>
       <c r="E111" t="n">
-        <v>0.8762197229717292</v>
+        <v>1.387982691457679</v>
       </c>
       <c r="F111" t="n">
         <v>0.06448425352573395</v>
@@ -18858,7 +18858,7 @@
         <v>1.098863005638123</v>
       </c>
       <c r="E112" t="n">
-        <v>0.8693937113938699</v>
+        <v>1.353768514999383</v>
       </c>
       <c r="F112" t="n">
         <v>-0.004998104181140661</v>
@@ -19025,7 +19025,7 @@
         <v>0.9648943543434143</v>
       </c>
       <c r="E113" t="n">
-        <v>0.8980519615179825</v>
+        <v>1.270657055567566</v>
       </c>
       <c r="F113" t="n">
         <v>-0.01641985960304737</v>
@@ -19192,7 +19192,7 @@
         <v>0.972774863243103</v>
       </c>
       <c r="E114" t="n">
-        <v>0.9362050951178754</v>
+        <v>1.288482306079544</v>
       </c>
       <c r="F114" t="n">
         <v>-0.05449239909648895</v>
@@ -19359,7 +19359,7 @@
         <v>1.169787645339966</v>
       </c>
       <c r="E115" t="n">
-        <v>0.9130181270178906</v>
+        <v>1.254797340568464</v>
       </c>
       <c r="F115" t="n">
         <v>0.03688168525695801</v>
@@ -19526,7 +19526,7 @@
         <v>1.228891372680664</v>
       </c>
       <c r="E116" t="n">
-        <v>0.9120484502137528</v>
+        <v>1.293150781510786</v>
       </c>
       <c r="F116" t="n">
         <v>0.03688168525695801</v>
@@ -19693,7 +19693,7 @@
         <v>1.150086283683777</v>
       </c>
       <c r="E117" t="n">
-        <v>0.9400079904741162</v>
+        <v>1.246326285225615</v>
       </c>
       <c r="F117" t="n">
         <v>0.1396775096654892</v>
@@ -19860,7 +19860,7 @@
         <v>1.055520176887512</v>
       </c>
       <c r="E118" t="n">
-        <v>0.9872716908376744</v>
+        <v>1.237782677617004</v>
       </c>
       <c r="F118" t="n">
         <v>-0.03260068595409393</v>
@@ -20027,7 +20027,7 @@
         <v>1.118564248085022</v>
       </c>
       <c r="E119" t="n">
-        <v>0.9896099767594285</v>
+        <v>1.222787701507213</v>
       </c>
       <c r="F119" t="n">
         <v>0.09018324315547943</v>
@@ -20194,7 +20194,7 @@
         <v>1.134325385093689</v>
       </c>
       <c r="E120" t="n">
-        <v>0.8913807281070817</v>
+        <v>1.209530089291889</v>
       </c>
       <c r="F120" t="n">
         <v>0.00737546244636178</v>
@@ -20361,7 +20361,7 @@
         <v>0.9806554317474365</v>
       </c>
       <c r="E121" t="n">
-        <v>0.8776737124368797</v>
+        <v>1.183202028677265</v>
       </c>
       <c r="F121" t="n">
         <v>0.1215930432081223</v>
@@ -20528,7 +20528,7 @@
         <v>1.1146240234375</v>
       </c>
       <c r="E122" t="n">
-        <v>0.8978573847530663</v>
+        <v>1.168916066955926</v>
       </c>
       <c r="F122" t="n">
         <v>-0.1582400500774384</v>
@@ -20695,7 +20695,7 @@
         <v>0.7678816318511963</v>
       </c>
       <c r="E123" t="n">
-        <v>0.9291939175400067</v>
+        <v>1.206386788664813</v>
       </c>
       <c r="F123" t="n">
         <v>-0.08304678648710251</v>
@@ -20862,7 +20862,7 @@
         <v>0.3620355725288391</v>
       </c>
       <c r="E124" t="n">
-        <v>0.8567763466368409</v>
+        <v>1.198185964224874</v>
       </c>
       <c r="F124" t="n">
         <v>-0.03831157088279724</v>
@@ -21029,7 +21029,7 @@
         <v>0.5590482354164124</v>
       </c>
       <c r="E125" t="n">
-        <v>0.7197423609194913</v>
+        <v>1.159547887074701</v>
       </c>
       <c r="F125" t="n">
         <v>-0.06781777739524841</v>
@@ -21196,7 +21196,7 @@
         <v>0.7008973360061646</v>
       </c>
       <c r="E126" t="n">
-        <v>0.5746833585714106</v>
+        <v>1.090878955050771</v>
       </c>
       <c r="F126" t="n">
         <v>-0.0411670058965683</v>
@@ -21363,7 +21363,7 @@
         <v>0.7324193716049194</v>
       </c>
       <c r="E127" t="n">
-        <v>0.5274318028262517</v>
+        <v>0.9706723633206475</v>
       </c>
       <c r="F127" t="n">
         <v>-0.004046292509883642</v>
@@ -21530,7 +21530,7 @@
         <v>0.7797024250030518</v>
       </c>
       <c r="E128" t="n">
-        <v>0.4806154029533465</v>
+        <v>0.869241929950932</v>
       </c>
       <c r="F128" t="n">
         <v>0.009279085323214531</v>
@@ -21697,7 +21697,7 @@
         <v>0.7954634428024292</v>
       </c>
       <c r="E129" t="n">
-        <v>0.3589793738653989</v>
+        <v>0.7866031643027839</v>
       </c>
       <c r="F129" t="n">
         <v>0.05115886032581329</v>
@@ -21864,7 +21864,7 @@
         <v>0.2989915013313293</v>
       </c>
       <c r="E130" t="n">
-        <v>0.2516555935516021</v>
+        <v>0.7298914765656624</v>
       </c>
       <c r="F130" t="n">
         <v>0.132063016295433</v>
@@ -22031,7 +22031,7 @@
         <v>0.5905702114105225</v>
       </c>
       <c r="E131" t="n">
-        <v>0.1465789882345123</v>
+        <v>0.5931155771328235</v>
       </c>
       <c r="F131" t="n">
         <v>0.224388912320137</v>
@@ -22198,7 +22198,7 @@
         <v>0.5275261998176575</v>
       </c>
       <c r="E132" t="n">
-        <v>0.1194992493447217</v>
+        <v>0.5121654391832279</v>
       </c>
       <c r="F132" t="n">
         <v>0.08161689341068268</v>
@@ -22365,7 +22365,7 @@
         <v>0.1413813382387161</v>
       </c>
       <c r="E133" t="n">
-        <v>0.1449581942757418</v>
+        <v>0.4544533450772311</v>
       </c>
       <c r="F133" t="n">
         <v>0.07590602338314056</v>
@@ -22532,7 +22532,7 @@
         <v>0.0231737308204174</v>
       </c>
       <c r="E134" t="n">
-        <v>0.1317095065148476</v>
+        <v>0.3937945249250882</v>
       </c>
       <c r="F134" t="n">
         <v>0.04354438185691833</v>
@@ -22699,7 +22699,7 @@
         <v>-0.9067261815071106</v>
       </c>
       <c r="E135" t="n">
-        <v>-0.1176838599271165</v>
+        <v>0.3596798712487394</v>
       </c>
       <c r="F135" t="n">
         <v>-0.03831157088279724</v>
@@ -22866,7 +22866,7 @@
         <v>-0.9382482171058655</v>
       </c>
       <c r="E136" t="n">
-        <v>-0.4179988227055674</v>
+        <v>0.09294983860189159</v>
       </c>
       <c r="F136" t="n">
         <v>0.004520027432590723</v>
@@ -23033,7 +23033,7 @@
         <v>-0.8042795658111572</v>
       </c>
       <c r="E137" t="n">
-        <v>-0.5751251595176339</v>
+        <v>-0.2407557929878798</v>
       </c>
       <c r="F137" t="n">
         <v>0.0235562901943922</v>
@@ -23200,7 +23200,7 @@
         <v>-0.8791444301605225</v>
       </c>
       <c r="E138" t="n">
-        <v>-0.6053607379586921</v>
+        <v>-0.438123980042194</v>
       </c>
       <c r="F138" t="n">
         <v>0.09684593975543976</v>
@@ -23367,7 +23367,7 @@
         <v>-0.7175940275192261</v>
       </c>
       <c r="E139" t="n">
-        <v>-0.6407205041785453</v>
+        <v>-0.6398015088122294</v>
       </c>
       <c r="F139" t="n">
         <v>0.1482438296079636</v>
@@ -23534,7 +23534,7 @@
         <v>-1.19042444229126</v>
       </c>
       <c r="E140" t="n">
-        <v>-0.7393335438019508</v>
+        <v>-0.7254479338949427</v>
       </c>
       <c r="F140" t="n">
         <v>0.1539546996355057</v>
@@ -23701,7 +23701,7 @@
         <v>-1.024933815002441</v>
       </c>
       <c r="E141" t="n">
-        <v>-0.8229243739288526</v>
+        <v>-0.631683436014543</v>
       </c>
       <c r="F141" t="n">
         <v>0.1901236027479172</v>
@@ -23868,7 +23868,7 @@
         <v>-0.7097135186195374</v>
       </c>
       <c r="E142" t="n">
-        <v>-0.6779335076216613</v>
+        <v>-0.5344104577693997</v>
       </c>
       <c r="F142" t="n">
         <v>0.2786422371864319</v>
@@ -24035,7 +24035,7 @@
         <v>-0.9382482171058655</v>
       </c>
       <c r="E143" t="n">
-        <v>-0.5112898381907129</v>
+        <v>-0.4721237592977533</v>
       </c>
       <c r="F143" t="n">
         <v>0.1939308792352676</v>
@@ -24202,7 +24202,7 @@
         <v>-0.8279210925102234</v>
       </c>
       <c r="E144" t="n">
-        <v>-0.6092251450185134</v>
+        <v>-0.3728041236947548</v>
       </c>
       <c r="F144" t="n">
         <v>0.2462805956602097</v>
@@ -24369,7 +24369,7 @@
         <v>-0.7333550453186035</v>
       </c>
       <c r="E145" t="n">
-        <v>-0.6571407117177095</v>
+        <v>-0.4078492338924456</v>
       </c>
       <c r="F145" t="n">
         <v>0.2396179288625717</v>
@@ -24536,7 +24536,7 @@
         <v>-0.6151474118232727</v>
       </c>
       <c r="E146" t="n">
-        <v>-0.6220031762423309</v>
+        <v>-0.226742585726521</v>
       </c>
       <c r="F146" t="n">
         <v>0.3538354635238647</v>
@@ -24703,7 +24703,7 @@
         <v>-0.5836253762245178</v>
       </c>
       <c r="E147" t="n">
-        <v>-0.603597139585519</v>
+        <v>-0.162318013823761</v>
       </c>
       <c r="F147" t="n">
         <v>0.3785826563835144</v>
@@ -24870,7 +24870,7 @@
         <v>-0.8318613767623901</v>
       </c>
       <c r="E148" t="n">
-        <v>-0.565842044539309</v>
+        <v>-0.2694477694007506</v>
       </c>
       <c r="F148" t="n">
         <v>0.5127882957458496</v>
@@ -25037,7 +25037,7 @@
         <v>-1.158902525901794</v>
       </c>
       <c r="E149" t="n">
-        <v>-0.4646761114949902</v>
+        <v>-0.3655817033604869</v>
       </c>
       <c r="F149" t="n">
         <v>0.6336686015129089</v>
@@ -25204,7 +25204,7 @@
         <v>-0.6781914830207825</v>
       </c>
       <c r="E150" t="n">
-        <v>-0.367936655273724</v>
+        <v>-0.5419067366198654</v>
       </c>
       <c r="F150" t="n">
         <v>0.6460421681404114</v>
@@ -25371,7 +25371,7 @@
         <v>-0.5245215892791748</v>
       </c>
       <c r="E151" t="n">
-        <v>-0.2722553843634145</v>
+        <v>-0.563272169682279</v>
       </c>
       <c r="F151" t="n">
         <v>0.4642458558082581</v>
@@ -25538,7 +25538,7 @@
         <v>-0.7097135186195374</v>
       </c>
       <c r="E152" t="n">
-        <v>-0.1696327017133998</v>
+        <v>-0.6876120850224935</v>
       </c>
       <c r="F152" t="n">
         <v>0.4147515296936035</v>
@@ -25705,7 +25705,7 @@
         <v>-0.7215343117713928</v>
       </c>
       <c r="E153" t="n">
-        <v>-0.2430124838977048</v>
+        <v>-0.7111387869930236</v>
       </c>
       <c r="F153" t="n">
         <v>0.354787290096283</v>
@@ -25872,7 +25872,7 @@
         <v>-1.08403754234314</v>
       </c>
       <c r="E154" t="n">
-        <v>-0.3143803076338668</v>
+        <v>-0.7362205258597144</v>
       </c>
       <c r="F154" t="n">
         <v>0.4366432428359985</v>
@@ -26039,7 +26039,7 @@
         <v>-1.103738903999329</v>
       </c>
       <c r="E155" t="n">
-        <v>-0.2650606968698634</v>
+        <v>-0.7760050339571348</v>
       </c>
       <c r="F155" t="n">
         <v>0.2681723237037659</v>
@@ -26206,7 +26206,7 @@
         <v>-1.099798679351807</v>
       </c>
       <c r="E156" t="n">
-        <v>-0.2293836984966721</v>
+        <v>-0.7806335530681023</v>
       </c>
       <c r="F156" t="n">
         <v>0.2491360157728195</v>
@@ -26373,7 +26373,7 @@
         <v>-0.8318613767623901</v>
       </c>
       <c r="E157" t="n">
-        <v>-0.2858140621945969</v>
+        <v>-0.7251781761589834</v>
       </c>
       <c r="F157" t="n">
         <v>0.3157629370689392</v>
@@ -26540,7 +26540,7 @@
         <v>-0.871263861656189</v>
       </c>
       <c r="E158" t="n">
-        <v>-0.3877711566674057</v>
+        <v>-0.6689091623912201</v>
       </c>
       <c r="F158" t="n">
         <v>0.3290883302688599</v>
@@ -26707,7 +26707,7 @@
         <v>-1.024933815002441</v>
       </c>
       <c r="E159" t="n">
-        <v>-0.5428872962638676</v>
+        <v>-0.6549318106698971</v>
       </c>
       <c r="F159" t="n">
         <v>0.4052333831787109</v>
@@ -26874,7 +26874,7 @@
         <v>-1.174663424491882</v>
       </c>
       <c r="E160" t="n">
-        <v>-0.5824052536457718</v>
+        <v>-0.6013944422821703</v>
       </c>
       <c r="F160" t="n">
         <v>0.4280769824981689</v>
@@ -27041,7 +27041,7 @@
         <v>-1.513525247573853</v>
       </c>
       <c r="E161" t="n">
-        <v>-0.5769738227937072</v>
+        <v>-0.6437039269504173</v>
       </c>
       <c r="F161" t="n">
         <v>0.5403909087181091</v>
@@ -27208,7 +27208,7 @@
         <v>-1.939072608947754</v>
       </c>
       <c r="E162" t="n">
-        <v>-0.5197349219253836</v>
+        <v>-0.640051340962157</v>
       </c>
       <c r="F162" t="n">
         <v>0.4290287494659424</v>
@@ -27375,7 +27375,7 @@
         <v>-1.48594343662262</v>
       </c>
       <c r="E163" t="n">
-        <v>-0.496750942447215</v>
+        <v>-0.6347532380419562</v>
       </c>
       <c r="F163" t="n">
         <v>0.3205220103263855</v>
@@ -27542,7 +27542,7 @@
         <v>-0.9185469150543213</v>
       </c>
       <c r="E164" t="n">
-        <v>-0.472745132652129</v>
+        <v>-0.6702780343793646</v>
       </c>
       <c r="F164" t="n">
         <v>0.2910158336162567</v>
@@ -27709,7 +27709,7 @@
         <v>-0.4063139259815216</v>
       </c>
       <c r="E165" t="n">
-        <v>-0.4943733836685593</v>
+        <v>-0.6656427332087715</v>
       </c>
       <c r="F165" t="n">
         <v>0.3071966767311096</v>
@@ -27876,7 +27876,7 @@
         <v>-0.2881063222885132</v>
       </c>
       <c r="E166" t="n">
-        <v>-0.5453529166694442</v>
+        <v>-0.6019335897353494</v>
       </c>
       <c r="F166" t="n">
         <v>0.3110039234161377</v>
@@ -28043,7 +28043,7 @@
         <v>-0.2684050500392914</v>
       </c>
       <c r="E167" t="n">
-        <v>-0.5607567090245704</v>
+        <v>-0.5064823042500941</v>
       </c>
       <c r="F167" t="n">
         <v>0.4299805760383606</v>
@@ -28210,7 +28210,7 @@
         <v>-0.2959868311882019</v>
       </c>
       <c r="E168" t="n">
-        <v>-0.5688432373588822</v>
+        <v>-0.3834395235308996</v>
       </c>
       <c r="F168" t="n">
         <v>0.5337282419204712</v>
@@ -28377,7 +28377,7 @@
         <v>-0.04381058365106583</v>
       </c>
       <c r="E169" t="n">
-        <v>-0.4539073574399289</v>
+        <v>-0.4140843125230858</v>
       </c>
       <c r="F169" t="n">
         <v>0.4699566960334778</v>
@@ -28544,7 +28544,7 @@
         <v>0.1689631193876266</v>
       </c>
       <c r="E170" t="n">
-        <v>-0.3773553062963487</v>
+        <v>-0.432157239646661</v>
       </c>
       <c r="F170" t="n">
         <v>0.4061852097511292</v>
@@ -28711,7 +28711,7 @@
         <v>0.2201864123344421</v>
       </c>
       <c r="E171" t="n">
-        <v>-0.3282780095851686</v>
+        <v>-0.4466237408467141</v>
       </c>
       <c r="F171" t="n">
         <v>0.4280769824981689</v>
@@ -28878,7 +28878,7 @@
         <v>0.4566016495227814</v>
       </c>
       <c r="E172" t="n">
-        <v>-0.3083671443030674</v>
+        <v>-0.4409551482041776</v>
       </c>
       <c r="F172" t="n">
         <v>0.4185587763786316</v>
@@ -29045,7 +29045,7 @@
         <v>0.4999444186687469</v>
       </c>
       <c r="E173" t="n">
-        <v>-0.249961992049676</v>
+        <v>-0.373247060534641</v>
       </c>
       <c r="F173" t="n">
         <v>0.4937520623207092</v>
@@ -29212,7 +29212,7 @@
         <v>0.7166584134101868</v>
       </c>
       <c r="E174" t="n">
-        <v>-0.1476889272020642</v>
+        <v>-0.3333084051595297</v>
       </c>
       <c r="F174" t="n">
         <v>0.4366432428359985</v>
@@ -29379,7 +29379,7 @@
         <v>0.9097307920455933</v>
       </c>
       <c r="E175" t="n">
-        <v>0.008904722200051902</v>
+        <v>-0.3492069724226878</v>
       </c>
       <c r="F175" t="n">
         <v>0.4176070094108582</v>
@@ -29546,7 +29546,7 @@
         <v>0.9924761652946472</v>
       </c>
       <c r="E176" t="n">
-        <v>0.127231507068283</v>
+        <v>-0.3416712104188981</v>
       </c>
       <c r="F176" t="n">
         <v>0.409992516040802</v>
@@ -29713,7 +29713,7 @@
         <v>0.91367107629776</v>
       </c>
       <c r="E177" t="n">
-        <v>0.1891934290024341</v>
+        <v>-0.2689570164117989</v>
       </c>
       <c r="F177" t="n">
         <v>0.4423540830612183</v>
@@ -29880,7 +29880,7 @@
         <v>1.248592615127563</v>
       </c>
       <c r="E178" t="n">
-        <v>0.2133088032336415</v>
+        <v>-0.1901907016616327</v>
       </c>
       <c r="F178" t="n">
         <v>0.470908522605896</v>
@@ -30047,7 +30047,7 @@
         <v>1.102803230285645</v>
       </c>
       <c r="E179" t="n">
-        <v>0.2389619569108384</v>
+        <v>-0.1337513740786989</v>
       </c>
       <c r="F179" t="n">
         <v>0.4747157692909241</v>
@@ -30214,7 +30214,7 @@
         <v>1.161907076835632</v>
       </c>
       <c r="E180" t="n">
-        <v>0.2779998995648648</v>
+        <v>-0.02254231478514785</v>
       </c>
       <c r="F180" t="n">
         <v>0.5089810490608215</v>
@@ -30381,7 +30381,7 @@
         <v>1.000356674194336</v>
       </c>
       <c r="E181" t="n">
-        <v>0.2454162827054591</v>
+        <v>0.1921800850818021</v>
       </c>
       <c r="F181" t="n">
         <v>0.4471132159233093</v>
@@ -30548,7 +30548,7 @@
         <v>0.9018502831459045</v>
       </c>
       <c r="E182" t="n">
-        <v>0.2090384977913463</v>
+        <v>0.4269053286286433</v>
       </c>
       <c r="F182" t="n">
         <v>0.449016809463501</v>
@@ -30715,7 +30715,7 @@
         <v>0.8821490406990051</v>
       </c>
       <c r="E183" t="n">
-        <v>0.1077109125157586</v>
+        <v>0.5465343412343766</v>
       </c>
       <c r="F183" t="n">
         <v>0.4299805760383606</v>
@@ -30882,7 +30882,7 @@
         <v>0.5472274422645569</v>
       </c>
       <c r="E184" t="n">
-        <v>0.04765386214835665</v>
+        <v>0.5880371814000273</v>
       </c>
       <c r="F184" t="n">
         <v>0.4461613893508911</v>
@@ -31049,7 +31049,7 @@
         <v>0.8506270051002502</v>
       </c>
       <c r="E185" t="n">
-        <v>-0.09408139867038152</v>
+        <v>0.6256494326012556</v>
       </c>
       <c r="F185" t="n">
         <v>0.4423540830612183</v>
@@ -31216,7 +31216,7 @@
         <v>1.544111728668213</v>
       </c>
       <c r="E186" t="n">
-        <v>-0.1828051438776121</v>
+        <v>0.6189069087031279</v>
       </c>
       <c r="F186" t="n">
         <v>0.4014261364936829</v>
@@ -31383,7 +31383,7 @@
         <v>1.559872627258301</v>
       </c>
       <c r="E187" t="n">
-        <v>-0.1578690878576066</v>
+        <v>0.600212608225177</v>
       </c>
       <c r="F187" t="n">
         <v>0.5042219758033752</v>
@@ -31550,7 +31550,7 @@
         <v>1.15796685218811</v>
       </c>
       <c r="E188" t="n">
-        <v>-0.05816115305399212</v>
+        <v>0.5885977265141954</v>
       </c>
       <c r="F188" t="n">
         <v>0.5499089956283569</v>
@@ -31717,7 +31717,7 @@
         <v>1.485007882118225</v>
       </c>
       <c r="E189" t="n">
-        <v>-0.04785009601897115</v>
+        <v>0.5880690413080357</v>
       </c>
       <c r="F189" t="n">
         <v>0.5299209356307983</v>
@@ -31884,7 +31884,7 @@
         <v>1.831750154495239</v>
       </c>
       <c r="E190" t="n">
-        <v>-0.1356739302602276</v>
+        <v>0.5174033973265943</v>
       </c>
       <c r="F190" t="n">
         <v>0.6498494148254395</v>
@@ -32051,7 +32051,7 @@
         <v>1.953898072242737</v>
       </c>
       <c r="E191" t="n">
-        <v>-0.1776700601154263</v>
+        <v>0.4034217111376724</v>
       </c>
       <c r="F191" t="n">
         <v>0.6812592744827271</v>
@@ -32218,7 +32218,7 @@
         <v>1.894794344902039</v>
       </c>
       <c r="E192" t="n">
-        <v>-0.1063091235871012</v>
+        <v>0.406532888986212</v>
       </c>
       <c r="F192" t="n">
         <v>0.7735852003097534</v>
@@ -32385,7 +32385,7 @@
         <v>1.646558284759521</v>
       </c>
       <c r="E193" t="n">
-        <v>-0.04527789475776729</v>
+        <v>0.4804281865632177</v>
       </c>
       <c r="F193" t="n">
         <v>0.949670672416687</v>
@@ -32552,7 +32552,7 @@
         <v>1.504709124565125</v>
       </c>
       <c r="E194" t="n">
-        <v>-0.03049137497677802</v>
+        <v>0.4366314593080128</v>
       </c>
       <c r="F194" t="n">
         <v>0.9353934526443481</v>
@@ -32719,7 +32719,7 @@
         <v>1.335278153419495</v>
       </c>
       <c r="E195" t="n">
-        <v>-0.1074630200573472</v>
+        <v>0.479527802430293</v>
       </c>
       <c r="F195" t="n">
         <v>1.027719378471375</v>
@@ -32886,7 +32886,7 @@
         <v>1.335278153419495</v>
       </c>
       <c r="E196" t="n">
-        <v>-0.1434167422354929</v>
+        <v>0.4185795881137402</v>
       </c>
       <c r="F196" t="n">
         <v>1.004875779151917</v>
@@ -33053,7 +33053,7 @@
         <v>1.595334887504578</v>
       </c>
       <c r="E197" t="n">
-        <v>-0.05792463529631402</v>
+        <v>0.3877607262578313</v>
       </c>
       <c r="F197" t="n">
         <v>0.9677550792694092</v>
@@ -33220,7 +33220,7 @@
         <v>1.764765977859497</v>
       </c>
       <c r="E198" t="n">
-        <v>0.008182491995798877</v>
+        <v>0.3996863472201063</v>
       </c>
       <c r="F198" t="n">
         <v>0.8478266000747681</v>

</xml_diff>